<commit_message>
Templater API descriptions and license
</commit_message>
<xml_diff>
--- a/FoodOrder/FoodOrder.Web/App_Data/Order.xlsx
+++ b/FoodOrder/FoodOrder.Web/App_Data/Order.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -30,7 +30,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>Templater formatting feature used beacuse Excel does not support multiple date values formatting in single cell.</t>
+          <t>Templater formatting feature used because Excel does not support multiple date values in a single cell.</t>
         </r>
       </text>
     </comment>
@@ -45,7 +45,7 @@
             <family val="2"/>
             <charset val="238"/>
           </rPr>
-          <t>This date field is using native Excel formatting capabilties.</t>
+          <t>This date field is using native Excel formatting features.</t>
         </r>
       </text>
     </comment>
@@ -149,8 +149,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,19 +296,19 @@
   </cellStyles>
   <dxfs count="23">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -329,22 +329,22 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -357,7 +357,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0"/>
@@ -372,7 +372,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0"/>
@@ -389,7 +389,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0"/>
@@ -406,7 +406,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0"/>
@@ -423,7 +423,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0"/>
@@ -436,7 +436,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
@@ -494,6 +494,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -614,6 +619,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -648,6 +654,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -823,34 +830,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.5703125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="7" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="9" customHeight="1"/>
-    <row r="2" spans="2:7" ht="18.75">
+    <row r="1" spans="2:7" ht="9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
     </row>
-    <row r="3" spans="2:7" ht="18.75">
+    <row r="3" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>18</v>
       </c>
@@ -860,7 +867,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>21</v>
       </c>
@@ -870,7 +877,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="2:7">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
@@ -880,7 +887,7 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="9" spans="2:7">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>0</v>
       </c>
@@ -897,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15" customHeight="1">
+    <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
@@ -917,7 +924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="2:7">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
@@ -937,7 +944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:7">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>28</v>
       </c>

</xml_diff>